<commit_message>
Updates to user story and product backlog documents
</commit_message>
<xml_diff>
--- a/Project Documents/Product Backlog.xlsx
+++ b/Project Documents/Product Backlog.xlsx
@@ -36,64 +36,64 @@
     <t>Story Points</t>
   </si>
   <si>
-    <t>As a player, I want to be able to spectate the game after I die so that I can see the other players' outcomes</t>
-  </si>
-  <si>
-    <t>As a player, I want to see a history of the effects on my character so that I can understand how my character developed into its current state</t>
-  </si>
-  <si>
-    <t>As a player, I want to review recent turns and actions so that I can see what players and NPCs have been doing</t>
-  </si>
-  <si>
-    <t>As a player, I want to see the special effects of an explored room before I enter it so that I can weigh the costs and benefits of traversing through</t>
-  </si>
-  <si>
-    <t>As a player, I want to play a tutorial to learn how to play the game.</t>
-  </si>
-  <si>
-    <t>As a player, I want to see my local gameplay stats (games played, times died, etc.) to see, in number form, how my games tend to go</t>
-  </si>
-  <si>
-    <t>As a player, I want to create a custom character (with stats) to add a bit of investment into the world and game</t>
-  </si>
-  <si>
-    <t>As a player, I want a place to view the character's info, likes and hobbies (character lore), to immerse myself more in the world and lore</t>
-  </si>
-  <si>
-    <t>As a player, I want the game elements to evolve as the phase changes in order to feel a difference between the peaceful Exploration Phase and the more chaotic Haunt Phase.</t>
-  </si>
-  <si>
-    <t>As a player, I want to be able to view the current state of the Haunt Timer at all times to be able to make tactical decisions about how to play</t>
+    <t>As a player, I want to spectate the game after death so that I can see the game’s outcome</t>
+  </si>
+  <si>
+    <t>As a player, I want to see past effects on my character so that I can understand its current state</t>
+  </si>
+  <si>
+    <t>As a player, I want to see recent actions so that I can understand others’ behavior</t>
+  </si>
+  <si>
+    <t>As a player, I want to see a room’s effects so that I can decide if I want to enter</t>
+  </si>
+  <si>
+    <t>As a player, I want to play a tutorial so that I can learn how to play the game.</t>
+  </si>
+  <si>
+    <t>As a player, I want to see my local gameplay stats (games played, times died, etc.) so that I can see, in number form, how my games tend to go</t>
+  </si>
+  <si>
+    <t>As a player, I want to create a custom character (with stats) so that I can create a bit of investment into the world and game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a player, I want a place to view the character lore, so that I can immerse myself more in the world and lore </t>
+  </si>
+  <si>
+    <t>As a player, I want the game elements to evolve as the phase changes so that I feel a difference between the peaceful Exploration Phase and the more chaotic Haunt Phase</t>
+  </si>
+  <si>
+    <t>As a player, I want to be able to view the current state of the Haunt Timer at so that I’m able to make tactical decisions about how to play</t>
   </si>
   <si>
     <t>As a player, I want to be able to change the volume in a settings menu to make the game experience more comfortable with my particular setup</t>
   </si>
   <si>
-    <t>As a player I want to be able to have an “inventory” of sorts to keep track of my items and what they do in order to know if I should use them</t>
-  </si>
-  <si>
-    <t>As a player I want to be able to view the board state of the game so that I can decide what my course of action will be and how I want to continue</t>
-  </si>
-  <si>
-    <t>As a player I want to be able to have an understandable ruleset that I can review to remember my win condition depending on the haunt</t>
-  </si>
-  <si>
-    <t>As a player I want to be able to keep track of my current stat points and that of others if necessary such that I can know how many dice to roll and if I need to reduce or add to my stats</t>
-  </si>
-  <si>
-    <t>As a player, I want to be able to have an accessibility option to change the size of font in the game.</t>
-  </si>
-  <si>
-    <t>As a player, I want to be able to have the option to invite friends to my game to play local multiplayer.</t>
-  </si>
-  <si>
-    <t>As a player, I want to be able to have a menu for custom modifiers/house rules before setting up the game.</t>
-  </si>
-  <si>
-    <t>As a player, I want to be able to have the ability to pause the game when I am playing with NPCs.</t>
-  </si>
-  <si>
-    <t>As a player, I want to be able to return to the main menu after a game so that I can browse the app quickly and conveniently</t>
+    <t>As a player, I want to be able to have an “inventory” to keep track of my items and what they do</t>
+  </si>
+  <si>
+    <t>As a player, I want to be able to view the board state so that I can decide what my course of action will be</t>
+  </si>
+  <si>
+    <t>As a player, I want to have a reviewable ruleset to remember my win/loss condition</t>
+  </si>
+  <si>
+    <t>As a player I want to be able to keep track of current stat points for users so I can know how many dice to roll and if I will die</t>
+  </si>
+  <si>
+    <t>As a player, I want to have the option to change the size of the font in the game</t>
+  </si>
+  <si>
+    <t>As a player, I want to be able to invite friends to my game to play local multiplayer</t>
+  </si>
+  <si>
+    <t>As a player, I want to have a menu for modifiers/house rules before setting up the game</t>
+  </si>
+  <si>
+    <t>As a player, I want to be able to have the ability to pause the game when playing with NPCs</t>
+  </si>
+  <si>
+    <t>As a player, I want to be able to return to the main menu after a game so that I can navigate easily</t>
   </si>
 </sst>
 </file>
@@ -129,12 +129,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -157,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -178,7 +184,13 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,7 +550,9 @@
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="7">
+        <v>2.0</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
@@ -562,7 +576,9 @@
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="8">
+        <v>1.0</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
@@ -574,7 +590,9 @@
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="7">
+        <v>2.0</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="5"/>
@@ -586,7 +604,9 @@
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="7">
+        <v>2.0</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
@@ -622,7 +642,9 @@
       <c r="B18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="7">
+        <v>2.0</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="5"/>
@@ -634,7 +656,9 @@
       <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="7">
+        <v>2.0</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
@@ -655,10 +679,12 @@
       <c r="A21" s="6">
         <v>20.0</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="7">
+        <v>1.0</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>

</xml_diff>

<commit_message>
Added some updated docs to /'Project Documents'
</commit_message>
<xml_diff>
--- a/Project Documents/Product Backlog.xlsx
+++ b/Project Documents/Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -39,13 +39,25 @@
     <t>As a player, I want to spectate the game after death so that I can see the game’s outcome</t>
   </si>
   <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
     <t>As a player, I want to see past effects on my character so that I can understand its current state</t>
   </si>
   <si>
+    <t>Low</t>
+  </si>
+  <si>
     <t>As a player, I want to see recent actions so that I can understand others’ behavior</t>
   </si>
   <si>
     <t>As a player, I want to see a room’s effects so that I can decide if I want to enter</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
   <si>
     <t>As a player, I want to play a tutorial so that I can learn how to play the game.</t>
@@ -100,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -127,6 +139,11 @@
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -176,21 +193,24 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,380 +462,526 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="6">
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="6">
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="6">
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="6">
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6">
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6">
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6">
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6">
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6">
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6">
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6">
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5">
+        <v>21.0</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6">
         <v>13.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4">
         <v>2.0</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6">
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="6">
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="6">
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="5">
+        <v>89.0</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="6">
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="6">
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="6">
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="6">
         <v>20.0</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="5"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="5"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="5"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="5"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added updated updated documents to /'Project Documents'
</commit_message>
<xml_diff>
--- a/Project Documents/Product Backlog.xlsx
+++ b/Project Documents/Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>As a player, I want to be able to view the board state so that I can decide what my course of action will be</t>
+  </si>
+  <si>
+    <t>DEVELOPING</t>
   </si>
   <si>
     <t>As a player, I want to have a reviewable ruleset to remember my win/loss condition</t>
@@ -709,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F14" s="5">
         <v>34.0</v>
@@ -720,7 +723,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="4">
         <v>3.0</v>
@@ -740,7 +743,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4">
         <v>3.0</v>
@@ -760,7 +763,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4">
         <v>5.0</v>
@@ -780,7 +783,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4">
         <v>5.0</v>
@@ -800,7 +803,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4">
         <v>5.0</v>
@@ -820,7 +823,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4">
         <v>3.0</v>
@@ -840,7 +843,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4">
         <v>2.0</v>

</xml_diff>

<commit_message>
Updated to current state (broken) for submission to Deliverable 2 as proof of work
</commit_message>
<xml_diff>
--- a/Project Documents/Product Backlog.xlsx
+++ b/Project Documents/Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -39,27 +39,15 @@
     <t>As a player, I want to spectate the game after death so that I can see the game’s outcome</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>As a player, I want to see past effects on my character so that I can understand its current state</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>As a player, I want to see recent actions so that I can understand others’ behavior</t>
   </si>
   <si>
     <t>As a player, I want to see a room’s effects so that I can decide if I want to enter</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>As a player, I want to play a tutorial so that I can learn how to play the game.</t>
   </si>
   <si>
@@ -85,9 +73,6 @@
   </si>
   <si>
     <t>As a player, I want to be able to view the board state so that I can decide what my course of action will be</t>
-  </si>
-  <si>
-    <t>DEVELOPING</t>
   </si>
   <si>
     <t>As a player, I want to have a reviewable ruleset to remember my win/loss condition</t>
@@ -115,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -142,11 +127,6 @@
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -183,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -196,24 +176,21 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,526 +442,380 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="6">
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5">
-        <v>55.0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="6">
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <v>34.0</v>
-      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="6">
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5">
-        <v>13.0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="6">
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="5">
-        <v>55.0</v>
-      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6">
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5">
-        <v>13.0</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6">
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="5">
-        <v>55.0</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6">
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="5">
-        <v>34.0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6">
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="5">
-        <v>34.0</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6">
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="5">
-        <v>13.0</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6">
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="5">
-        <v>13.0</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6">
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="5">
-        <v>21.0</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6">
         <v>13.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7">
         <v>2.0</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="5">
-        <v>34.0</v>
-      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6">
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="5">
-        <v>13.0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="6">
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="5">
-        <v>34.0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="6">
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="5">
-        <v>89.0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="6">
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="5">
-        <v>55.0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="6">
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="5">
-        <v>55.0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="6">
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="5">
-        <v>13.0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="6">
         <v>20.0</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="5">
-        <v>8.0</v>
-      </c>
+      <c r="B21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="10"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="10"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added Architectural Design Doc, Use Case Doc, etc
</commit_message>
<xml_diff>
--- a/Project Documents/Product Backlog.xlsx
+++ b/Project Documents/Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -39,15 +39,27 @@
     <t>As a player, I want to spectate the game after death so that I can see the game’s outcome</t>
   </si>
   <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
     <t>As a player, I want to see past effects on my character so that I can understand its current state</t>
   </si>
   <si>
+    <t>Low</t>
+  </si>
+  <si>
     <t>As a player, I want to see recent actions so that I can understand others’ behavior</t>
   </si>
   <si>
     <t>As a player, I want to see a room’s effects so that I can decide if I want to enter</t>
   </si>
   <si>
+    <t>High</t>
+  </si>
+  <si>
     <t>As a player, I want to play a tutorial so that I can learn how to play the game.</t>
   </si>
   <si>
@@ -73,6 +85,9 @@
   </si>
   <si>
     <t>As a player, I want to be able to view the board state so that I can decide what my course of action will be</t>
+  </si>
+  <si>
+    <t>DEVELOPING</t>
   </si>
   <si>
     <t>As a player, I want to have a reviewable ruleset to remember my win/loss condition</t>
@@ -100,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -127,6 +142,11 @@
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -176,21 +196,24 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,380 +465,526 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="6">
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="6">
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="6">
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="6">
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6">
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6">
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6">
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6">
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6">
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6">
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6">
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5">
+        <v>21.0</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6">
         <v>13.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4">
         <v>2.0</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6">
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="6">
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="5">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="6">
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="5">
+        <v>89.0</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="6">
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="6">
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="6">
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="6">
         <v>20.0</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
+      <c r="B21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="5"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="5"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="5"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="5"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>

</xml_diff>